<commit_message>
Add New Project xm-la
</commit_message>
<xml_diff>
--- a/TEMPLATE/Testcase-template-xm-web-v2.xlsx
+++ b/TEMPLATE/Testcase-template-xm-web-v2.xlsx
@@ -96,13 +96,13 @@
     <t>Site is Opened</t>
   </si>
   <si>
-    <t>XM DEV website</t>
-  </si>
-  <si>
     <t>ERP user/ pass: superuser/ superuser</t>
   </si>
   <si>
     <t>Can login with ERP account</t>
+  </si>
+  <si>
+    <t>XM DEV V2 website https://hk-dev.xm-dev.int.iptp.net/</t>
   </si>
 </sst>
 </file>
@@ -339,6 +339,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -347,6 +356,69 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -370,80 +442,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -752,7 +752,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:E18"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -766,47 +766,47 @@
       <c r="A1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="33"/>
       <c r="C1" s="1">
         <v>43</v>
       </c>
       <c r="D1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="28"/>
-      <c r="F1" s="18" t="s">
+      <c r="E1" s="33"/>
+      <c r="F1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="28"/>
+      <c r="B2" s="33"/>
       <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="28"/>
-      <c r="F2" s="18" t="s">
+      <c r="E2" s="33"/>
+      <c r="F2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="35" t="s">
+      <c r="G2" s="22"/>
+      <c r="H2" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="28"/>
-      <c r="J2" s="36" t="s">
+      <c r="I2" s="33"/>
+      <c r="J2" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="37"/>
+      <c r="K2" s="36"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
@@ -822,10 +822,10 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="39"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="10"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -850,31 +850,31 @@
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="39"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="40">
+      <c r="E6" s="38"/>
+      <c r="F6" s="39">
         <f ca="1">TODAY()</f>
-        <v>45176</v>
-      </c>
-      <c r="G6" s="41"/>
-      <c r="H6" s="35" t="s">
+        <v>45236</v>
+      </c>
+      <c r="G6" s="40"/>
+      <c r="H6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="39"/>
-      <c r="J6" s="34" t="str">
+      <c r="I6" s="38"/>
+      <c r="J6" s="31" t="str">
         <f>IF(COUNTIF(I18:I34,"Fail")&gt;0, "Fail", "Pass")</f>
         <v>Pass</v>
       </c>
-      <c r="K6" s="34"/>
+      <c r="K6" s="31"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
@@ -893,11 +893,11 @@
       <c r="A8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
       <c r="E8" s="7"/>
       <c r="F8" s="12" t="s">
         <v>8</v>
@@ -905,78 +905,78 @@
       <c r="G8" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-    </row>
-    <row r="9" spans="1:11" ht="13" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+    </row>
+    <row r="9" spans="1:11" ht="24.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8">
         <v>1</v>
       </c>
-      <c r="B9" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="22"/>
+      <c r="B9" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="45"/>
+      <c r="D9" s="46"/>
       <c r="E9" s="3"/>
       <c r="F9" s="8">
         <v>1</v>
       </c>
-      <c r="G9" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="19"/>
+      <c r="G9" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="22"/>
     </row>
     <row r="10" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8">
         <v>2</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
+      <c r="B10" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="45"/>
+      <c r="D10" s="46"/>
       <c r="E10" s="3"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="19"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="22"/>
     </row>
     <row r="11" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8">
         <v>3</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="22"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="46"/>
       <c r="E11" s="3"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="19"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="22"/>
     </row>
     <row r="12" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8">
         <v>4</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="46"/>
       <c r="E12" s="3"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="19"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="22"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
@@ -1007,40 +1007,40 @@
       <c r="K14" s="4"/>
     </row>
     <row r="16" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="26" t="s">
+      <c r="C16" s="48"/>
+      <c r="D16" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="23" t="s">
+      <c r="E16" s="51"/>
+      <c r="F16" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="23" t="s">
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="24"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
+      <c r="A17" s="48"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
     </row>
     <row r="18" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
@@ -1054,16 +1054,16 @@
         <v>23</v>
       </c>
       <c r="E18" s="15"/>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="17" t="s">
+      <c r="G18" s="21"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="J18" s="18"/>
-      <c r="K18" s="19"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="22"/>
     </row>
     <row r="19" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
@@ -1074,28 +1074,28 @@
       <c r="C19" s="16"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="19"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="22"/>
     </row>
     <row r="20" spans="1:11" s="14" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13">
         <f t="shared" ref="A20:A22" si="0">A19+1</f>
         <v>3</v>
       </c>
-      <c r="B20" s="45"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="52"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="30"/>
     </row>
     <row r="21" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
@@ -1106,12 +1106,12 @@
       <c r="C21" s="16"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="19"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="22"/>
     </row>
     <row r="22" spans="1:11" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
@@ -1122,31 +1122,34 @@
       <c r="C22" s="16"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="19"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:E17"/>
+    <mergeCell ref="F16:H17"/>
+    <mergeCell ref="I16:K17"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
@@ -1161,25 +1164,22 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="D16:E17"/>
-    <mergeCell ref="F16:H17"/>
-    <mergeCell ref="I16:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:K22"/>
   </mergeCells>
   <conditionalFormatting sqref="J6:K6">
     <cfRule type="expression" dxfId="2" priority="3">

</xml_diff>